<commit_message>
Refactor get_schedule_course function and update schedule.html template
</commit_message>
<xml_diff>
--- a/static/schedule-courses/Horario 1-2024 - 2771132.xlsx
+++ b/static/schedule-courses/Horario 1-2024 - 2771132.xlsx
@@ -475,7 +475,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:G32"/>
+  <dimension ref="A2:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -520,6 +520,16 @@
           <t>2771132</t>
         </is>
       </c>
+      <c r="D5" s="1" t="inlineStr">
+        <is>
+          <t>Instructor titular:</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DANIEL DAVID BENAVIDES SÁNCHEZ </t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -1017,22 +1027,22 @@
     <row r="29">
       <c r="A29" s="6" t="inlineStr">
         <is>
-          <t>Emprendimiento</t>
+          <t>Instalación + Manual de Usuario</t>
         </is>
       </c>
       <c r="B29" s="6" t="inlineStr">
         <is>
-          <t>Fomentar cultura emprendedora según habilidades y competencias personales.</t>
+          <t>Desarrollar la solución de software de acuerdo con el diseño y metodologías de desarrollo.</t>
         </is>
       </c>
       <c r="C29" s="6" t="inlineStr">
         <is>
-          <t>Fomentar cultura emprendedora según habilidades y competencias personales.</t>
+          <t>Desarrollo de la solución de software.</t>
         </is>
       </c>
       <c r="D29" s="6" t="inlineStr">
         <is>
-          <t>Establecer características y competencias emprendedoras personales de acuerdo con sus potencialidades, objetivos y el entorno.</t>
+          <t>Codificar el software empleando el lenguaje de programación seleccionado.</t>
         </is>
       </c>
     </row>
@@ -1054,7 +1064,7 @@
       </c>
       <c r="D30" s="6" t="inlineStr">
         <is>
-          <t>Apropiar el proceso de toma de decisiones personales en su cotidianidad, según el comportamiento emprendedor.</t>
+          <t>Establecer características y competencias emprendedoras personales de acuerdo con sus potencialidades, objetivos y el entorno.</t>
         </is>
       </c>
     </row>
@@ -1076,7 +1086,7 @@
       </c>
       <c r="D31" s="6" t="inlineStr">
         <is>
-          <t>Emplear capacidad creativa e innovadora según estrategia emprendedora.</t>
+          <t>Apropiar el proceso de toma de decisiones personales en su cotidianidad, según el comportamiento emprendedor.</t>
         </is>
       </c>
     </row>
@@ -1097,6 +1107,28 @@
         </is>
       </c>
       <c r="D32" s="6" t="inlineStr">
+        <is>
+          <t>Emplear capacidad creativa e innovadora según estrategia emprendedora.</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="6" t="inlineStr">
+        <is>
+          <t>Emprendimiento</t>
+        </is>
+      </c>
+      <c r="B33" s="6" t="inlineStr">
+        <is>
+          <t>Fomentar cultura emprendedora según habilidades y competencias personales.</t>
+        </is>
+      </c>
+      <c r="C33" s="6" t="inlineStr">
+        <is>
+          <t>Fomentar cultura emprendedora según habilidades y competencias personales.</t>
+        </is>
+      </c>
+      <c r="D33" s="6" t="inlineStr">
         <is>
           <t>Establecer características y competencias emprendedoras personales de acuerdo con sus potencialidades, objetivos y el entorno.</t>
         </is>

</xml_diff>